<commit_message>
Added ability to use protein tags in beta_gb version
</commit_message>
<xml_diff>
--- a/ProteinTags.xlsx
+++ b/ProteinTags.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nixon\CASdesigner_Working\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -19,52 +24,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
-  <si>
-    <t>N</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>MBP</t>
-  </si>
-  <si>
-    <t>atgtctAAGATTGAAGAAGGTAAGTTGGTTATCTGGATTAACGGTGACAAGGGTTACAACGGTTTGGCTGAAGTTGGTAAGAAATTTGAAAAAGATACCGGTATCAAGGTCACTGTTGAACACCCAGACAAGTTGGAAGAAAAGTTTCCACAAGTTGCTGCCACTGGTGATGGTCCAGACATTATCTTCTGGGCTCATGACAGATTCGGTGGTTACGCCCAATCCGGTTTGTTAGCCGAGATCACCCCAGATAAGGCTTTTCAAGATAAGTTGTATCCATTCACTTGGGATGCCGTCAGATACAACGGTAAGTTAATCGCCTACCCAATTGCTGTTGAAGCTTTGTCTTTGATCTACAATAAGGACTTGTTACCTAACCCACCAAAGACCTGGGAAGAAATCCCAGCTTTAGATAAGGAGTTAAAAGCTAAGGGTAAGTCCGCTTTGATGTTTAACTTGCAAGAACCATACTTCACTTGGCCATTGATCGCTGCTGATGGTGGTTACGCTTTTAAGTATGAAAACGGTAAATACGACATTAAGGATGTCGGTGTCGACAATGCTGGTGCTAAGGCCGGTTTAACTTTCTTAGTCGATTTGATTAAGAATAAACATATGAATGCTGACACTGATTACTCTATTGCTGAAGCTGCTTTCAACAAGGGTGAAACCGCTATGACTATTAACGGTCCATGGGCCTGGTCTAACATTGATACCTCTAAAGTCAACTACGGTGTCACCGTCTTGCCAACTTTTAAGGGTCAACCATCTAAGCCATTCGTCGGTGTCTTGTCTGCCGGTATTAACGCTGCCTCTCCAAATAAGGAATTGGCCAAGGAATTCTTAGAAAACTACTTGTTAACCGATGAAGGTTTAGAGGCCGTTAACAAGGATAAGCCATTAGGTGCTGTTGCTTTGAAGTCTTACGAAGAAGAGTTGGCTAAGGATCCAAGAATTGCTGCTACTATGGAAAACGCTCAAAAGGGTGAAATTATGCCAAACATCCCACAAATGTCTGCTTTCTGGTACGCTGTTCGTACCGCCGTCATTAATGCCGCTTCTGGTCGTCAAACTGTTGATGAAGCCTTGAAGGACGCTCAAACCAGAATTACTAAGggaggtggtggaggtgga</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>GGTAGCGGTAGCGGCAGCtctAAGATTGAAGAAGGTAAGTTGGTTATCTGGATTAACGGTGACAAGGGTTACAACGGTTTGGCTGAAGTTGGTAAGAAATTTGAAAAAGATACCGGTATCAAGGTCACTGTTGAACACCCAGACAAGTTGGAAGAAAAGTTTCCACAAGTTGCTGCCACTGGTGATGGTCCAGACATTATCTTCTGGGCTCATGACAGATTCGGTGGTTACGCCCAATCCGGTTTGTTAGCCGAGATCACCCCAGATAAGGCTTTTCAAGATAAGTTGTATCCATTCACTTGGGATGCCGTCAGATACAACGGTAAGTTAATCGCCTACCCAATTGCTGTTGAAGCTTTGTCTTTGATCTACAATAAGGACTTGTTACCTAACCCACCAAAGACCTGGGAAGAAATCCCAGCTTTAGATAAGGAGTTAAAAGCTAAGGGTAAGTCCGCTTTGATGTTTAACTTGCAAGAACCATACTTCACTTGGCCATTGATCGCTGCTGATGGTGGTTACGCTTTTAAGTATGAAAACGGTAAATACGACATTAAGGATGTCGGTGTCGACAATGCTGGTGCTAAGGCCGGTTTAACTTTCTTAGTCGATTTGATTAAGAATAAACATATGAATGCTGACACTGATTACTCTATTGCTGAAGCTGCTTTCAACAAGGGTGAAACCGCTATGACTATTAACGGTCCATGGGCCTGGTCTAACATTGATACCTCTAAAGTCAACTACGGTGTCACCGTCTTGCCAACTTTTAAGGGTCAACCATCTAAGCCATTCGTCGGTGTCTTGTCTGCCGGTATTAACGCTGCCTCTCCAAATAAGGAATTGGCCAAGGAATTCTTAGAAAACTACTTGTTAACCGATGAAGGTTTAGAGGCCGTTAACAAGGATAAGCCATTAGGTGCTGTTGCTTTGAAGTCTTACGAAGAAGAGTTGGCTAAGGATCCAAGAATTGCTGCTACTATGGAAAACGCTCAAAAGGGTGAAATTATGCCAAACATCCCACAAATGTCTGCTTTCTGGTACGCTGTTCGTACCGCCGTCATTAATGCCGCTTCTGGTCGTCAAACTGTTGATGAAGCCTTGAAGGACGCTCAAACCAGAATTACTAAGtaa</t>
-  </si>
-  <si>
-    <t>terminus</t>
-  </si>
-  <si>
-    <t>name</t>
   </si>
   <si>
     <t>sequence</t>
   </si>
   <si>
-    <t>Fixed_Fprimer</t>
+    <t>tagName</t>
   </si>
   <si>
-    <t>Fixed_Rprimer</t>
-  </si>
-  <si>
-    <t>tccacctccaccacctccCTTAGTAATTCTGGTTTGAGCGTCC</t>
-  </si>
-  <si>
-    <t>GGTAGCGGTAGCGGCAGCAAGATTGAAGAAGGTAAGTTGGTTATCTGG</t>
-  </si>
-  <si>
-    <t>custom</t>
+    <t>AAGATTGAAGAAGGTAAGTTGGTTATCTGGATTAACGGTGACAAGGGTTACAACGGTTTGGCTGAAGTTGGTAAGAAATTTGAAAAAGATACCGGTATCAAGGTCACTGTTGAACACCCAGACAAGTTGGAAGAAAAGTTTCCACAAGTTGCTGCCACTGGTGATGGTCCAGACATTATCTTCTGGGCTCATGACAGATTCGGTGGTTACGCCCAATCCGGTTTGTTAGCCGAGATCACCCCAGATAAGGCTTTTCAAGATAAGTTGTATCCATTCACTTGGGATGCCGTCAGATACAACGGTAAGTTAATCGCCTACCCAATTGCTGTTGAAGCTTTGTCTTTGATCTACAATAAGGACTTGTTACCTAACCCACCAAAGACCTGGGAAGAAATCCCAGCTTTAGATAAGGAGTTAAAAGCTAAGGGTAAGTCCGCTTTGATGTTTAACTTGCAAGAACCATACTTCACTTGGCCATTGATCGCTGCTGATGGTGGTTACGCTTTTAAGTATGAAAACGGTAAATACGACATTAAGGATGTCGGTGTCGACAATGCTGGTGCTAAGGCCGGTTTAACTTTCTTAGTCGATTTGATTAAGAATAAACATATGAATGCTGACACTGATTACTCTATTGCTGAAGCTGCTTTCAACAAGGGTGAAACCGCTATGACTATTAACGGTCCATGGGCCTGGTCTAACATTGATACCTCTAAAGTCAACTACGGTGTCACCGTCTTGCCAACTTTTAAGGGTCAACCATCTAAGCCATTCGTCGGTGTCTTGTCTGCCGGTATTAACGCTGCCTCTCCAAATAAGGAATTGGCCAAGGAATTCTTAGAAAACTACTTGTTAACCGATGAAGGTTTAGAGGCCGTTAACAAGGATAAGCCATTAGGTGCTGTTGCTTTGAAGTCTTACGAAGAAGAGTTGGCTAAGGATCCAAGAATTGCTGCTACTATGGAAAACGCTCAAAAGGGTGAAATTATGCCAAACATCCCACAAATGTCTGCTTTCTGGTACGCTGTTCGTACCGCCGTCATTAATGCCGCTTCTGGTCGTCAAACTGTTGATGAAGCCTTGAAGGACGCTCAAACCAGAATTACTAAG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,6 +97,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -444,64 +430,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
+    <row r="3" spans="1:2" ht="16.5">
+      <c r="B3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
protein tags fix ength
</commit_message>
<xml_diff>
--- a/ProteinTags.xlsx
+++ b/ProteinTags.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nixon\CASdesigner_Working\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-200" windowWidth="28800" windowHeight="12220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>MBP</t>
   </si>
@@ -35,25 +30,75 @@
     <t>tagName</t>
   </si>
   <si>
-    <t>AAGATTGAAGAAGGTAAGTTGGTTATCTGGATTAACGGTGACAAGGGTTACAACGGTTTGGCTGAAGTTGGTAAGAAATTTGAAAAAGATACCGGTATCAAGGTCACTGTTGAACACCCAGACAAGTTGGAAGAAAAGTTTCCACAAGTTGCTGCCACTGGTGATGGTCCAGACATTATCTTCTGGGCTCATGACAGATTCGGTGGTTACGCCCAATCCGGTTTGTTAGCCGAGATCACCCCAGATAAGGCTTTTCAAGATAAGTTGTATCCATTCACTTGGGATGCCGTCAGATACAACGGTAAGTTAATCGCCTACCCAATTGCTGTTGAAGCTTTGTCTTTGATCTACAATAAGGACTTGTTACCTAACCCACCAAAGACCTGGGAAGAAATCCCAGCTTTAGATAAGGAGTTAAAAGCTAAGGGTAAGTCCGCTTTGATGTTTAACTTGCAAGAACCATACTTCACTTGGCCATTGATCGCTGCTGATGGTGGTTACGCTTTTAAGTATGAAAACGGTAAATACGACATTAAGGATGTCGGTGTCGACAATGCTGGTGCTAAGGCCGGTTTAACTTTCTTAGTCGATTTGATTAAGAATAAACATATGAATGCTGACACTGATTACTCTATTGCTGAAGCTGCTTTCAACAAGGGTGAAACCGCTATGACTATTAACGGTCCATGGGCCTGGTCTAACATTGATACCTCTAAAGTCAACTACGGTGTCACCGTCTTGCCAACTTTTAAGGGTCAACCATCTAAGCCATTCGTCGGTGTCTTGTCTGCCGGTATTAACGCTGCCTCTCCAAATAAGGAATTGGCCAAGGAATTCTTAGAAAACTACTTGTTAACCGATGAAGGTTTAGAGGCCGTTAACAAGGATAAGCCATTAGGTGCTGTTGCTTTGAAGTCTTACGAAGAAGAGTTGGCTAAGGATCCAAGAATTGCTGCTACTATGGAAAACGCTCAAAAGGGTGAAATTATGCCAAACATCCCACAAATGTCTGCTTTCTGGTACGCTGTTCGTACCGCCGTCATTAATGCCGCTTCTGGTCGTCAAACTGTTGATGAAGCCTTGAAGGACGCTCAAACCAGAATTACTAAG</t>
+    <t>GFP</t>
+  </si>
+  <si>
+    <t>PX1</t>
+  </si>
+  <si>
+    <t>mCherry</t>
+  </si>
+  <si>
+    <t>COX4</t>
+  </si>
+  <si>
+    <t>ERG20</t>
+  </si>
+  <si>
+    <t>UbiX</t>
+  </si>
+  <si>
+    <t>CYB5</t>
+  </si>
+  <si>
+    <t>SNC1</t>
+  </si>
+  <si>
+    <t>NES1</t>
+  </si>
+  <si>
+    <t>atgAAGATTGAAGAAGGTAAGTTGGTTATCTGGATTAACGGTGACAAGGGTTACAACGGTTTGGCTGAAGTTGGTAAGAAATTTGAAAAAGATACCGGTATCAAGGTCACTGTTGAACACCCAGACAAGTTGGAAGAAAAGTTTCCACAAGTTGCTGCCACTGGTGATGGTCCAGACATTATCTTCTGGGCTCATGACAGATTCGGTGGTTACGCCCAATCCGGTTTGTTAGCCGAGATCACCCCAGATAAGGCTTTTCAAGATAAGTTGTATCCATTCACTTGGGATGCCGTCAGATACAACGGTAAGTTAATCGCCTACCCAATTGCTGTTGAAGCTTTGTCTTTGATCTACAATAAGGACTTGTTACCTAACCCACCAAAGACCTGGGAAGAAATCCCAGCTTTAGATAAGGAGTTAAAAGCTAAGGGTAAGTCCGCTTTGATGTTTAACTTGCAAGAACCATACTTCACTTGGCCATTGATCGCTGCTGATGGTGGTTACGCTTTTAAGTATGAAAACGGTAAATACGACATTAAGGATGTCGGTGTCGACAATGCTGGTGCTAAGGCCGGTTTAACTTTCTTAGTCGATTTGATTAAGAATAAACATATGAATGCTGACACTGATTACTCTATTGCTGAAGCTGCTTTCAACAAGGGTGAAACCGCTATGACTATTAACGGTCCATGGGCCTGGTCTAACATTGATACCTCTAAAGTCAACTACGGTGTCACCGTCTTGCCAACTTTTAAGGGTCAACCATCTAAGCCATTCGTCGGTGTCTTGTCTGCCGGTATTAACGCTGCCTCTCCAAATAAGGAATTGGCCAAGGAATTCTTAGAAAACTACTTGTTAACCGATGAAGGTTTAGAGGCCGTTAACAAGGATAAGCCATTAGGTGCTGTTGCTTTGAAGTCTTACGAAGAAGAGTTGGCTAAGGATCCAAGAATTGCTGCTACTATGGAAAACGCTCAAAAGGGTGAAATTATGCCAAACATCCCACAAATGTCTGCTTTCTGGTACGCTGTTCGTACCGCCGTCATTAATGCCGCTTCTGGTCGTCAAACTGTTGATGAAGCCTTGAAGGACGCTCAAACCAGAATTACTAAGtaa</t>
+  </si>
+  <si>
+    <t>ATGtctaaaggtgaagaattattcactggtgttgtcccaattttggttgaattagatggtgatgttaatggtcacaaattttctgtctccggtgaaggtgaaggtgatgctacttacggtaaattgaccttaaaatttatttgtactactggtaaattgccagttccatggccaaccttagtcactactttcggttatggtgttcaatgttttgcgagatacccagatcatatgaaacaacatgactttttcaagtctgccatgccagaaggttatgttcaagaaagaactatttttttcaaagatgacggtaactacaagaccagagctgaagtcaagtttgaaggtgataccttagttaatagaatcgaattaaaaggtattgattttaaagaagatggtaacattttaggtcacaaattggaatacaactataactctcacaatgtttacatcatggctgacaaacaaaagaatggtatcaaagttaacttcaaaattagacacaacattgaagatggttctgttcaattagctgaccattatcaacaaaatactccaattggtgatggtccagtcttgttaccagacaaccattacttatccactcaatctgccttatccaaagatccaaacgaaaagagagaccacatggtcttgttagaatttgttactgctgctggtattatccatggtatggatgaattgtacaaaTAA</t>
+  </si>
+  <si>
+    <t>ATGTCTAAATTATAA</t>
+  </si>
+  <si>
+    <t>ATGtctatggttagtaaaggagaagaaaataacatggcaatcattaaggagttcatgagattcaaagttcacatggaaggttctgtaaatggacatgaatttgaaatagaaggtgaaggagaaggaaggccttatgaaggaacccaaaccgcgaagctaaaagttactaagggtggcccattaccatttgcatgggatatccttagccctcaattcatgtatgggtcaaaggcttatgtcaagcaccccgccgacattccagactatctaaagttatcttttcccgaagggtttaagtgggagcgtgtgatgaacttcgaagacggtggcgtggtaacagtgactcaggattcgtccctgcaagatggtgaatttatctacaaagtcaaattaagaggaactaactttccatctgacggcccggttatgcaaaaaaagacaatgggctgggaggcctcctcagaacgaatgtaccctgaagatggtgccttgaagggtgagattaaacaaagattgaaattgaaagatggtggacattatgacgctgaggttaaaacgacatacaaagctaagaaacctgtccagctcccaggtgcttacaatgtaaatataaaacttgatattacatcacataatgaagattatacgatagttgaacaatacgaaagggctgaggggagacatagtactggtggcatggatgaactatacaaaTAA</t>
+  </si>
+  <si>
+    <t>ATGCTTTCACTACGTCAATCTATAAGATTTTTCAAGCCAGCCACAAGAACTTTGTGTAGCTCTAGATAA</t>
+  </si>
+  <si>
+    <t>ATGGCTTCAGAAAAAGAAATTAGGAGAGAGAGATTCTTGAACGTTTTCCCTAAATTAGTAGAGGAATTGAACGCATCGCTTTTGGCTTACGGTATGCCTAAGGAAGCATGTGACTGGTATGCCCACTCATTGAACTACAACACTCCAGGCGGTAAGCTAAATAGAGGTTTGTCCGTTGTGGACACGTATGCTATTCTCTCCAACAAGACCGTTGAACAATTGGGGCAAGAAGAATACGAAAAGGTTGCCATTCTAGGTTGGTGCATTGAGTTGTTGCAGGCTTACTTCTTGGTCGCCGATGATATGATGGACAAGTCCATTACCAGAAGAGGCCAACCATGTTGGTACAAGGTTCCTGAAGTTGGGGAAATTGCCATCAATGACGCATTCATGTTAGAGGCTGCTATCTACAAGCTTTTGAAATCTCACTTCAGAAACGAAAAATACTACATAGATATCACCGAATTGTTCCATGAGGTCACCTTCCAAACCGAATTGGGCCAATTGATGGACTTAATCACTGCACCTGAAGACAAAGTCGACTTGAGTAAGTTCTCCCTAAAGAAGCACTCCTTCATAGTTACTTTCAAGACTGCTTACTATTCTTTCTACTTGCCTGTCGCATTGGCCATGTACGTTGCCGGTATCACGGATGAAAAGGATTTGAAACAAGCCAGAGATGTCTTGATTCCATTGGGTGAATACTTCCAAATTCAAGATGACTACTTAGACTGCTTCGGTACCCCAGAACAGATCGGTAAGATCGGTACAGATATCCAAGATAACAAATGTTCTTGGGTAATCAACAAGGCATTGGAACTTGCTTCCGCAGAACAAAGAAAGACTTTAGACGAAAATTACGGTAAGAAGGACTCAGTCGCAGAAGCCAAATGCAAAAAGATTTTCAATGACTTGAAAATTGAACAGCTATACCACGAATATGAAGAGTCTATTGCCAAGGATTTGAAGGCCAAAATTTCTCAGGTCGATGAGTCTCGTGGCTTCAAAGCTGATGTCTTAACTGCGTTCTTGAACAAAGTTTACAAGAGAAGCAAATAA</t>
+  </si>
+  <si>
+    <t>ATGCAGATTTTCGTCAAGACTTTGACCGGTAAAACCATAACATTGGAAGTTGAATCTTCCGATACCATCGACAACGTTAAGTCGAAAATTCAAGACAAGGAAGGTATCCCTCCAGATCAACAAAGATTGATCTTTGCCGGTAAGCAGCTAGAAGACGGTAGAACGCTGTCTGATTACAACATTCAGAAGGAGTCCACCTTACATCTTGTGCTAAGGCTAAGAGGTGGTTATCACGGATCCGGAGCTTGGCTGTTGCCCGTCTCACTGGTGAAAAGAAAAACCACCCTGGCGCCCAATACGTAA</t>
+  </si>
+  <si>
+    <t>ATGTCTACCTCTGAAAACCAAAGTAAAGGTAGTGGTACATTGGTTGTCATATTGGCCATTTTAATGCTAGGTGTTGCTTATTATTTGTTGAACGAATAA</t>
+  </si>
+  <si>
+    <t>ATGTGGTACAAGGATCTAAAAATGAAGATGTGTCTGGCTTTAGTAATCATCATATTGCTTGTTGTAATCATCGTCCCCATTGCTGTTCACTTTAGTCGATAA</t>
+  </si>
+  <si>
+    <t>ATGaacgagctggccctgaagctggccggactggacatcTAA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF212121"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
       <u/>
@@ -62,6 +107,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,18 +145,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -430,19 +511,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="11" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -450,12 +534,81 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5">
-      <c r="B3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>